<commit_message>
start php side ...
</commit_message>
<xml_diff>
--- a/name.xlsx
+++ b/name.xlsx
@@ -7,7 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Таблица умножения" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet 1" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -355,10 +356,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,40 +430,6 @@
       </c>
       <c r="E4" s="1">
         <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1">
-        <v>24</v>
-      </c>
-      <c r="E5" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -479,4 +446,32 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>